<commit_message>
summery of contents for brackets
</commit_message>
<xml_diff>
--- a/thesis-tex/excels/references.xlsx
+++ b/thesis-tex/excels/references.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E77D6E-766F-46B2-958B-FBB090A43072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AA378C-F6A5-498A-8F08-8BAA922B3830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{708375FB-6962-4B20-A84D-3D0BF229F98B}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Brackets" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -453,11 +454,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C99330B-41D4-434B-87B1-F3F6E5AC9A2D}">
   <dimension ref="B4:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1276,7 +1276,7 @@
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       <c r="E8">
         <v>1984</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>102</v>
       </c>
       <c r="G8" t="s">

</xml_diff>